<commit_message>
chore: modifying folder structure
</commit_message>
<xml_diff>
--- a/tooth_analysis/Age histogram.xlsx
+++ b/tooth_analysis/Age histogram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dropbox\AI Projects\buck\tooth_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222030C9-7EC4-4AFF-A630-77604EA571FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84D9208-A3F4-4676-BCDE-986864BEEBF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2F0F71B1-4197-4497-8392-3431E7EA0A26}"/>
   </bookViews>
@@ -33,6 +33,17 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Total (5.5+)</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -594,10 +605,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>33</c:v>
@@ -1830,10 +1841,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76DDA1E5-CE0D-4E97-B918-1B230963BD06}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1843,7 +1854,7 @@
         <v>0.5</v>
       </c>
       <c r="B1">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1851,7 +1862,7 @@
         <v>1.5</v>
       </c>
       <c r="B2">
-        <v>55</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1972,6 +1983,24 @@
       </c>
       <c r="B17">
         <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <f>SUM(B6:B17)</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <f>SUM(B1:B17)</f>
+        <v>243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>